<commit_message>
Modeling updates and figures
</commit_message>
<xml_diff>
--- a/tables/OSM_all_covariates_summary.xlsx
+++ b/tables/OSM_all_covariates_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,187 +467,187 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>lc_water</t>
+          <t>lc_coniferous</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0 (0–0.05)</t>
+          <t>0.45 (0.22–0.79)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.03 (0–0.68)</t>
+          <t>0.48 (0–1)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>lc_coniferous</t>
+          <t>lc_broadleaf</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.45 (0.22–0.79)</t>
+          <t>0.1 (0.01–0.31)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.48 (0–1)</t>
+          <t>0.17 (0–1)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>lc_broadleaf</t>
+          <t>lc_mixed</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.1 (0.01–0.31)</t>
+          <t>0.07 (0.01–0.17)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.17 (0–1)</t>
+          <t>0.11 (0–0.93)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>lc_mixed</t>
+          <t>lc_developed</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.07 (0.01–0.17)</t>
+          <t>0.02 (0–0.06)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.11 (0–0.93)</t>
+          <t>0.04 (0–0.56)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>lc_developed</t>
+          <t>lc_shrub</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.02 (0–0.06)</t>
+          <t>0.06 (0.01–0.2)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.04 (0–0.56)</t>
+          <t>0.13 (0–1)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lc_shrub</t>
+          <t>osm_industrial</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.06 (0.01–0.2)</t>
+          <t>0 (0–0.02)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.13 (0–1)</t>
+          <t>0.02 (0–0.69)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>osm_industrial</t>
+          <t>natural_cohesion</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0 (0–0.02)</t>
+          <t>99.57 (99.08–99.82)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.02 (0–0.69)</t>
+          <t>99.32 (50.56–100)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>seismic</t>
+          <t>anthropogenic_cohesion</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.01 (0–0.02)</t>
+          <t>99.72 (99.11–99.88)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.01 (0–0.1)</t>
+          <t>98.89 (61.4–100)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>pipe_trans</t>
+          <t>natural_ed</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.01 (0–0.03)</t>
+          <t>73.88 (44.89–131.19)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.02 (0–0.46)</t>
+          <t>98.49 (0–597.03)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>anthropogenic_cohesion</t>
+          <t>anthropogenic_ed</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>99.7 (98.98–99.87)</t>
+          <t>71.85 (43.4–128.41)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>96.93 (0–100)</t>
+          <t>96.57 (0–597.03)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>anthropogenic_ed</t>
+          <t>natural_tca</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>71.85 (43.4–128.41)</t>
+          <t>1351.06 (227.22–3562.92)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>96.57 (0–597.03)</t>
+          <t>1909.32 (0–7620.17)</t>
         </is>
       </c>
     </row>
@@ -671,51 +671,340 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>natural_cohesion</t>
+          <t>natural_cai_mn</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>99.57 (99.08–99.82)</t>
+          <t>37.87 (23.02–58.18)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>99.32 (50.56–100)</t>
+          <t>40.95 (0–98.57)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>natural_ed</t>
+          <t>anthro_cai_mn</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>73.88 (44.89–131.19)</t>
+          <t>2.46 (0.85–7.42)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>98.49 (0–597.03)</t>
+          <t>6.72 (0–90.58)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>natural_tca</t>
+          <t>forest_cai_mn</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1351.06 (227.22–3562.92)</t>
+          <t>39.37 (25.08–53.52)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1909.32 (0–7620.17)</t>
+          <t>39.95 (0–97.8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>nonforest_cai_mn</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>20.96 (8.12–40.1)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>24.6 (0–91.85)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>nonveg_anthro_cai_mn</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>4.01 (0.85–9.45)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>7.07 (0–87.3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>veg_anthro_cai_mn</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2.09 (0.69–4.36)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3.49 (0–90.49)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>forest_cohesion</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>99.47 (98.93–99.76)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>99.2 (72.43–100)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>nonforest_cohesion</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>98.32 (96.83–99.13)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>97.72 (0–100)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>nonveg_anthro_cohesion</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>98.77 (97.43–99.43)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>98.03 (34.43–100)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>veg_anthro_cohesion</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>99.31 (98.24–99.7)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>98.39 (61.4–100)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>forest_ed</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>68.44 (45.78–108.18)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>91.01 (0–597.03)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>nonforest_ed</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>26.77 (8.86–50.99)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>33.94 (0–275.53)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>nonveg_anthro_ed</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>23.7 (6.29–47.93)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>31.41 (0–387.89)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>veg_anthro_ed</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>85.3 (49.61–154.26)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>109.24 (0–602.17)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>forest_tca</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1031.99 (165.01–2888.4)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1545.25 (0–7333.05)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>nonforest_tca</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>80.83 (8.08–393.89)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>274.52 (0–4339.95)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>nonveg_anthro_tca</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>6.65 (0.07–45.38)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>40.24 (0–2075.66)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>veg_anthro_tca</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>33.78 (1.78–208.87)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>138.77 (0–2137.73)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>seismic</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.02)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>pipe_trans</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.03)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.02 (0–0.46)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Final figures and tables (for now)
</commit_message>
<xml_diff>
--- a/tables/OSM_all_covariates_summary.xlsx
+++ b/tables/OSM_all_covariates_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,7 +365,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Median (20%, 80%)</t>
+          <t>Median (5%, 95% quantiles)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -376,550 +376,803 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>UglyName</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>CFI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.05 (0.05–0.23)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.07 (0–1)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>cfi_site</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.05 (0.02–0.11)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.07 (0–0.73)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>CFI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.06 (0.06–0.28)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.09 (0–1)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>cfi_site_with_harvest</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.06 (0.02–0.14)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.09 (0–0.79)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>CFI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.06 (0.06–0.26)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.08 (0–1)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>cfi_site_with_vegedges</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.06 (0.02–0.12)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.08 (0–0.73)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Fire &lt;15</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0 (0–0.74)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.07 (0–1)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>fire_0_15</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0 (0–0)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.07 (0–1)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Harvest &lt;15</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0 (0–0.12)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.02 (0–1)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>harvest_0_15</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0 (0–0.01)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.02 (0–0.79)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Harvest</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0 (0–0.28)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.05 (0–1)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>harvest_total</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0 (0–0.09)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0.05 (0–0.92)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>landscape_mesh</t>
+          <t>Core Area Index</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>130.86 (42.57–316.3)</t>
+          <t>0 (0–0)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>211.93 (0.95–2978.46)</t>
+          <t>0 (0–0)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>landscape_cai_mn</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>landscape_np</t>
+          <t>Contagion</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>417 (88–1268)</t>
+          <t>62.84 (62.84–80.38)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>890.35 (1–16279)</t>
+          <t>63.54 (18.38–99.53)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>landscape_contag</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>landscape_shei</t>
+          <t>Edge Density</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.64 (0.53–0.74)</t>
+          <t>0 (0–0)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.63 (0–1)</t>
+          <t>0 (0–0)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>landscape_ed</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>landscape_siei</t>
+          <t>Mesh Index</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.76 (0.62–0.84)</t>
+          <t>113.08 (113.08–651.94)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.72 (0–1)</t>
+          <t>192.78 (0.15–2978.46)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>landscape_mesh</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lc_broadleaf</t>
+          <t>Number of Patches</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.08 (0.02–0.27)</t>
+          <t>340 (340–2983)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.15 (0–0.94)</t>
+          <t>809.76 (1–16279)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>landscape_np</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>lc_coniferous</t>
+          <t>Shannon's Evenness</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.34 (0.22–0.47)</t>
+          <t>0.64 (0.64–0.87)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.35 (0–0.96)</t>
+          <t>0.62 (0–1)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>landscape_shei</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>lc_herbs</t>
+          <t>Simpson's Evenness</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.02 (0–0.05)</t>
+          <t>0.75 (0.75–0.9)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.03 (0–0.37)</t>
+          <t>0.7 (0–1)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>landscape_siei</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>lc_mixedwood</t>
+          <t>Total Core Area</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.05 (0.01–0.11)</t>
+          <t>0 (0–0)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.07 (0–0.67)</t>
+          <t>0 (0–0)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>landscape_tca</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>lc_shrubs</t>
+          <t>Broadleaf</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0 (0–0.01)</t>
+          <t>0.08 (0.08–0.52)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.03 (0–0.92)</t>
+          <t>0.15 (0–1)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>lc_broadleaf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>lc_wetland</t>
+          <t>Coniferous</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.04 (0.01–0.11)</t>
+          <t>0.34 (0.34–0.67)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.07 (0–0.62)</t>
+          <t>0.35 (0–1)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>lc_coniferous</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>lc_wetland_treed</t>
+          <t>Herbs</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.23 (0.1–0.4)</t>
+          <t>0.01 (0.01–0.13)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.25 (0–0.93)</t>
+          <t>0.03 (0–0.43)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>lc_herbs</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>nonanthro_cai_mn</t>
+          <t>Mixedwood</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>18.48 (6.58–36.91)</t>
+          <t>0.05 (0.05–0.21)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23.84 (0–96.43)</t>
+          <t>0.07 (0–0.71)</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>lc_mixedwood</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>nonanthro_ed</t>
+          <t>Shrubland</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>73.88 (44.89–131.19)</t>
+          <t>0 (0–0.2)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>98.49 (0–597.03)</t>
+          <t>0.03 (0–0.96)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>lc_shrubs</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>nonanthro_tca</t>
+          <t>Wetland</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>979.07 (139.96–2836.5)</t>
+          <t>0.04 (0.04–0.24)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1520.97 (0–7439.42)</t>
+          <t>0.07 (0–0.76)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>lc_wetland</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>osm_industrial</t>
+          <t>Treed Wetland</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0 (0–0.02)</t>
+          <t>0.23 (0.23–0.6)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.02 (0–0.69)</t>
+          <t>0.25 (0–0.95)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>lc_wetland_treed</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>pct_lari_lar</t>
+          <t>Core Area Index (natural habitat)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0.01 (0–0.04)</t>
+          <t>32.73 (32.73–84.77)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.02 (0–0.41)</t>
+          <t>36.34 (0–98.21)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>nonanthro_cai_mn</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>pct_pice_gla</t>
+          <t>Edge Density</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0 (0–0.01)</t>
+          <t>74.6 (74.6–296.57)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.01 (0–0.31)</t>
+          <t>101.65 (0–742.03)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>nonanthro_ed</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>pct_pice_mar</t>
+          <t>Total Core Area (natural)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.56 (0.25–0.77)</t>
+          <t>1024.54 (1024.54–5263.56)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.52 (0–0.99)</t>
+          <t>1664.25 (0–7585.52)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>nonanthro_tca</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>pct_pinu_ban</t>
+          <t>Industrial Facilities</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0.01 (0–0.05)</t>
+          <t>0 (0–0.09)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.06 (0–1)</t>
+          <t>0.02 (0–1)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>osm_industrial</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>pct_popu_tre</t>
+          <t>Tamarack</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0.33 (0.14–0.6)</t>
+          <t>0 (0–0.09)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.36 (0–1)</t>
+          <t>0.02 (0–0.47)</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>pct_lari_lar</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>pipe_trans</t>
+          <t>White Spruce</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.01 (0–0.03)</t>
+          <t>0 (0–0.06)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.02 (0–0.46)</t>
+          <t>0.01 (0–0.39)</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>pct_pice_gla</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>roads</t>
+          <t>Black Spruce</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0 (0–0.01)</t>
+          <t>0.56 (0.56–0.9)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.01 (0–0.07)</t>
+          <t>0.52 (0–1)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>pct_pice_mar</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>seismic</t>
+          <t>Jack Pine</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.01 (0–0.02)</t>
+          <t>0.01 (0.01–0.55)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.01 (0–0.1)</t>
+          <t>0.07 (0–1)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>pct_pinu_ban</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>wells_active</t>
+          <t>Trembling Aspen</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0 (0–0.01)</t>
+          <t>0.32 (0.32–0.8)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0 (0–0.19)</t>
+          <t>0.36 (0–1)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>pct_popu_tre</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>wells_inactive</t>
+          <t>Pipelines &amp; Transmission Lines</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0 (0–0.01)</t>
+          <t>0.01 (0.01–0.07)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.01 (0–0.3)</t>
+          <t>0.02 (0–0.46)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>pipe_trans</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>Roads</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>0 (0–0.02)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.12)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>roads</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Seismic Lines</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>0.01 (0.01–0.04)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.2)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>seismic</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Active Well Sites</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>0 (0–0.03)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.32)</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>wells_active</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Inactive Well Sites</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>0 (0–0.02)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.59)</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>wells_inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Well Sites</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0 (0–0.05)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.01 (0–0.59)</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>wells_total</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>0.01 (0–0.02)</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>0.01 (0–0.3)</t>
         </is>
       </c>
     </row>

</xml_diff>